<commit_message>
+ working project to store this state
</commit_message>
<xml_diff>
--- a/Ref.xlsx
+++ b/Ref.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MetaboApp-main\REPORT_METABOSCAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEC8BBD-7C49-475A-B753-B1EC92B334C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB2F608-BA9B-4EC8-BA83-AEB877FE6910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3BEB3553-591A-4AAE-BC2B-1E70F2790E13}"/>
   </bookViews>
@@ -1316,8 +1316,8 @@
   <dimension ref="A1:FI7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FF15" sqref="FF15"/>
+      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
+ streamlit app refact work
</commit_message>
<xml_diff>
--- a/Ref.xlsx
+++ b/Ref.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MetaboApp-main\REPORT_METABOSCAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E7585A-BAA2-40C8-A134-DD1276D83A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53FB4E2-7EB3-48CA-B912-66F9CABCF96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9300" yWindow="840" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref_stats" sheetId="1" r:id="rId1"/>
@@ -1692,7 +1692,7 @@
   </sheetPr>
   <dimension ref="A1:FI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="CK1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="CN21" sqref="CN21"/>
     </sheetView>
@@ -5369,8 +5369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E35516-F0CF-4D6A-BB44-A2C6B02294B4}">
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
+FINAL changes in REF and ENV
</commit_message>
<xml_diff>
--- a/Ref.xlsx
+++ b/Ref.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MetaboApp-main\REPORT_METABOSCAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4FC3D7-38E7-4B70-B0CD-A116779097C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD17DD39-D7BF-47B8-97D1-D7E572BD1808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="797" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref_stats" sheetId="1" r:id="rId1"/>
-    <sheet name="Group_score" sheetId="3" r:id="rId2"/>
+    <sheet name="metrics_ml_models" sheetId="3" r:id="rId2"/>
     <sheet name="Params_metaboscan" sheetId="2" r:id="rId3"/>
     <sheet name="Controls" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="433">
   <si>
     <t>metabolite</t>
   </si>
@@ -543,66 +543,9 @@
     <t>name_view</t>
   </si>
   <si>
-    <t>5-гидрокситриптофан</t>
-  </si>
-  <si>
-    <t>Антранилловая кислота</t>
-  </si>
-  <si>
-    <t>Аргинин</t>
-  </si>
-  <si>
-    <t>Цитруллин</t>
-  </si>
-  <si>
-    <t>Гомоаргинин</t>
-  </si>
-  <si>
-    <t>3-индолуксусная кислота</t>
-  </si>
-  <si>
-    <t>3-индолмасляная</t>
-  </si>
-  <si>
-    <t>3-индолкарбоксальдегид</t>
-  </si>
-  <si>
-    <t>3-индолмолочная кислота</t>
-  </si>
-  <si>
-    <t>3-индолпропионовая кислота</t>
-  </si>
-  <si>
-    <t>Кинуреновая кислота</t>
-  </si>
-  <si>
-    <t>Кинуренин</t>
-  </si>
-  <si>
     <t>Мелатонин</t>
   </si>
   <si>
-    <t>Орнитин</t>
-  </si>
-  <si>
-    <t>Хинолиновая кислота</t>
-  </si>
-  <si>
-    <t>Серин</t>
-  </si>
-  <si>
-    <t>Серотонин</t>
-  </si>
-  <si>
-    <t>Триптамин</t>
-  </si>
-  <si>
-    <t>Триптофан</t>
-  </si>
-  <si>
-    <t>Ксантуреновая кислота</t>
-  </si>
-  <si>
     <t>Аденозин</t>
   </si>
   <si>
@@ -612,78 +555,9 @@
     <t>Уридин</t>
   </si>
   <si>
-    <t>Аланин</t>
-  </si>
-  <si>
-    <t>Аспарагин</t>
-  </si>
-  <si>
-    <t>Аспарагиновая кислота</t>
-  </si>
-  <si>
-    <t>Глутамат</t>
-  </si>
-  <si>
-    <t>Глутамин</t>
-  </si>
-  <si>
-    <t>Глицин</t>
-  </si>
-  <si>
-    <t>Гистидин</t>
-  </si>
-  <si>
-    <t>Гидроксипролин</t>
-  </si>
-  <si>
-    <t>Лизин</t>
-  </si>
-  <si>
-    <t>Метилгистидин</t>
-  </si>
-  <si>
-    <t>Фенилаланин</t>
-  </si>
-  <si>
-    <t>Пролин</t>
-  </si>
-  <si>
-    <t>Сумма Leu-Ile</t>
-  </si>
-  <si>
-    <t>Таурин</t>
-  </si>
-  <si>
-    <t>Треонин</t>
-  </si>
-  <si>
-    <t>Тирозин</t>
-  </si>
-  <si>
-    <t>Валин</t>
-  </si>
-  <si>
-    <t>Бетаин</t>
-  </si>
-  <si>
-    <t>Холин</t>
-  </si>
-  <si>
-    <t>Метионин</t>
-  </si>
-  <si>
-    <t>Метионин сульфоксид</t>
-  </si>
-  <si>
-    <t>Карнозин</t>
-  </si>
-  <si>
     <t>Кортизол</t>
   </si>
   <si>
-    <t>Креатинин</t>
-  </si>
-  <si>
     <t>Гистамин</t>
   </si>
   <si>
@@ -693,9 +567,6 @@
     <t>Рибофлавин</t>
   </si>
   <si>
-    <t>SDMA</t>
-  </si>
-  <si>
     <t>Arg / ADMA</t>
   </si>
   <si>
@@ -1228,6 +1099,240 @@
   </si>
   <si>
     <t>MK62</t>
+  </si>
+  <si>
+    <t>5-гидрокситриптофан (5-HTP)</t>
+  </si>
+  <si>
+    <t>Асимметричный диметиларгинин (ADMA)</t>
+  </si>
+  <si>
+    <t>Антраниловая кислота (Ant)</t>
+  </si>
+  <si>
+    <t>Аргинин (Arg)</t>
+  </si>
+  <si>
+    <t>Цитруллин (Cit)</t>
+  </si>
+  <si>
+    <t>5-Гидроксииндолуксусная кислота (5-HIAA)</t>
+  </si>
+  <si>
+    <t>Гомоаргинин (HomoArg)</t>
+  </si>
+  <si>
+    <t>3-Индолуксусная кислота (IAA)</t>
+  </si>
+  <si>
+    <t>3-Индолмолочная кислота (ILA)</t>
+  </si>
+  <si>
+    <t>3-Индолкарбоксальдегид (ICAA)</t>
+  </si>
+  <si>
+    <t>3-Индолпропионовая кислота (IPA)</t>
+  </si>
+  <si>
+    <t>3-Индолмасляная кислота (IBA)</t>
+  </si>
+  <si>
+    <t>Кинуреновая кислота (Kyna)</t>
+  </si>
+  <si>
+    <t>Кинуренин (Kyn)</t>
+  </si>
+  <si>
+    <t>Монометиларгинин (MMA)</t>
+  </si>
+  <si>
+    <t>Орнитин (Orn)</t>
+  </si>
+  <si>
+    <t>Хинолиновая кислота (QA)</t>
+  </si>
+  <si>
+    <t>Серин (Ser)</t>
+  </si>
+  <si>
+    <t>Серотонин (Ser)</t>
+  </si>
+  <si>
+    <t>Триптамин (TA)</t>
+  </si>
+  <si>
+    <t>Триптофан (Trp)</t>
+  </si>
+  <si>
+    <t>Ксантуреновая кислота (Xnt)</t>
+  </si>
+  <si>
+    <t>Аланин (Ala)</t>
+  </si>
+  <si>
+    <t>Аспарагин (Asn)</t>
+  </si>
+  <si>
+    <t>Аспарагиновая кислота (Asp)</t>
+  </si>
+  <si>
+    <t>Глутаминовая кислота (Glu)</t>
+  </si>
+  <si>
+    <t>Глутамин (Gln)</t>
+  </si>
+  <si>
+    <t>Глицин (Gly)</t>
+  </si>
+  <si>
+    <t>Гистидин (His)</t>
+  </si>
+  <si>
+    <t>Гидроксипролин (Hyp)</t>
+  </si>
+  <si>
+    <t>Лизин (Lys)</t>
+  </si>
+  <si>
+    <t>Метилгистидин (MH)</t>
+  </si>
+  <si>
+    <t>Фенилаланин (Phe)</t>
+  </si>
+  <si>
+    <t>Пролин (Pro)</t>
+  </si>
+  <si>
+    <t>Лейцин + Изолейцин (Leu+Ile)</t>
+  </si>
+  <si>
+    <t>Таурин (Tau)</t>
+  </si>
+  <si>
+    <t>Треонин (Thr)</t>
+  </si>
+  <si>
+    <t>Тирозин (Tyr)</t>
+  </si>
+  <si>
+    <t>Валин (Val)</t>
+  </si>
+  <si>
+    <t>Бетаин (Bet)</t>
+  </si>
+  <si>
+    <t>Холин (Chl)</t>
+  </si>
+  <si>
+    <t>Диметилглицин (DMG)</t>
+  </si>
+  <si>
+    <t>Метионин (Met)</t>
+  </si>
+  <si>
+    <t>Метионин сульфоксид (MetSO)</t>
+  </si>
+  <si>
+    <t>Триметиламин-N-оксид (TMAO)</t>
+  </si>
+  <si>
+    <t>Карнозин (Car)</t>
+  </si>
+  <si>
+    <t>Креатинин (Cr)</t>
+  </si>
+  <si>
+    <t>Симметричный диметиларгинин (SDMA)</t>
+  </si>
+  <si>
+    <t>Карнитин (C0)</t>
+  </si>
+  <si>
+    <t>Деканоилкарнитин (C10)</t>
+  </si>
+  <si>
+    <t>Деценоилкарнитин (C10-1)</t>
+  </si>
+  <si>
+    <t>Декадиеноилкарнитин (C10-2)</t>
+  </si>
+  <si>
+    <t>Додеканоилкарнитин (C12)</t>
+  </si>
+  <si>
+    <t>Додеценоилкарнитин (C12-1)</t>
+  </si>
+  <si>
+    <t>Тетрадеканоилкарнитин (C14)</t>
+  </si>
+  <si>
+    <t>Тетрадеценоилкарнитин (С14-1)</t>
+  </si>
+  <si>
+    <t>Тетрадекадиеноилкарнитин (C14-2)</t>
+  </si>
+  <si>
+    <t>Гидрокситетрадеканоилкарнитин (C14-OH)</t>
+  </si>
+  <si>
+    <t>Пальмитоилкарнитин (C16)</t>
+  </si>
+  <si>
+    <t>Гексадецениолкарнитин (C16-1)</t>
+  </si>
+  <si>
+    <t>Гидроксигексадецениолкарнитин (C16-1-OH)</t>
+  </si>
+  <si>
+    <t>Гидроксигексадеканоилкарнитин (C16-OH)</t>
+  </si>
+  <si>
+    <t>Стеароилкарнитин (С18)</t>
+  </si>
+  <si>
+    <t>Олеоилкарнитин (C18-1)</t>
+  </si>
+  <si>
+    <t>Гидроксиоктадеценоилкарнитин (C18-1-OH)</t>
+  </si>
+  <si>
+    <t>Линолеоилкарнитин (C18-2)</t>
+  </si>
+  <si>
+    <t>Гидроксиоктадеканоилкарнитин (C18-OH)</t>
+  </si>
+  <si>
+    <t>Ацетилкарнитин (C2)</t>
+  </si>
+  <si>
+    <t>Пропионилкарнитин (С3)</t>
+  </si>
+  <si>
+    <t>Бутирилкарнитин (C4)</t>
+  </si>
+  <si>
+    <t>Изовалерилкарнитин (С5)</t>
+  </si>
+  <si>
+    <t>Тиглилкарнитин (C5-1)</t>
+  </si>
+  <si>
+    <t>Глутарилкарнитин (C5-DC)</t>
+  </si>
+  <si>
+    <t>Гидроксиизовалерилкарнитин (C5-OH)</t>
+  </si>
+  <si>
+    <t>Гексаноилкарнитин (C6)</t>
+  </si>
+  <si>
+    <t>Адипоилкарнитин (C6-DC)</t>
+  </si>
+  <si>
+    <t>Октаноилкарнитин (C8)</t>
+  </si>
+  <si>
+    <t>Октеноилкарнитин (C8-1)</t>
   </si>
 </sst>
 </file>
@@ -1890,8 +1995,8 @@
   <dimension ref="A1:FI6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FC8" sqref="FC8"/>
+      <pane xSplit="1" topLeftCell="FC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="FE12" sqref="FE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2261,7 +2366,7 @@
         <v>106</v>
       </c>
       <c r="DD1" s="2" t="s">
-        <v>258</v>
+        <v>215</v>
       </c>
       <c r="DE1" s="2" t="s">
         <v>107</v>
@@ -4756,289 +4861,289 @@
         <v>168</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="E6" t="s">
+        <v>358</v>
+      </c>
+      <c r="F6" t="s">
+        <v>359</v>
+      </c>
+      <c r="G6" t="s">
+        <v>360</v>
+      </c>
+      <c r="H6" t="s">
+        <v>361</v>
+      </c>
+      <c r="I6" t="s">
+        <v>362</v>
+      </c>
+      <c r="J6" t="s">
+        <v>366</v>
+      </c>
+      <c r="K6" t="s">
+        <v>364</v>
+      </c>
+      <c r="L6" t="s">
+        <v>363</v>
+      </c>
+      <c r="M6" t="s">
+        <v>365</v>
+      </c>
+      <c r="N6" t="s">
+        <v>367</v>
+      </c>
+      <c r="O6" t="s">
+        <v>368</v>
+      </c>
+      <c r="P6" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11" t="s">
+      <c r="Q6" t="s">
+        <v>369</v>
+      </c>
+      <c r="R6" t="s">
+        <v>370</v>
+      </c>
+      <c r="S6" t="s">
+        <v>371</v>
+      </c>
+      <c r="T6" t="s">
+        <v>372</v>
+      </c>
+      <c r="U6" t="s">
+        <v>373</v>
+      </c>
+      <c r="V6" t="s">
+        <v>374</v>
+      </c>
+      <c r="W6" t="s">
+        <v>375</v>
+      </c>
+      <c r="X6" t="s">
+        <v>376</v>
+      </c>
+      <c r="Y6" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="Z6" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="AA6" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="11" t="s">
+      <c r="AB6" t="s">
+        <v>377</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>378</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>379</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>380</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>381</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>382</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>383</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>384</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>385</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>386</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>387</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>388</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>389</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>390</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>391</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>392</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>393</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>394</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>395</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>396</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>397</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>398</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>399</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>400</v>
+      </c>
+      <c r="AZ6" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="BA6" t="s">
+        <v>401</v>
+      </c>
+      <c r="BB6" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="BC6" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="BD6" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="BE6" t="s">
+        <v>402</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>403</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>404</v>
+      </c>
+      <c r="BH6" t="s">
+        <v>405</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>406</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>407</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>408</v>
+      </c>
+      <c r="BL6" t="s">
+        <v>409</v>
+      </c>
+      <c r="BM6" t="s">
+        <v>410</v>
+      </c>
+      <c r="BN6" t="s">
+        <v>411</v>
+      </c>
+      <c r="BO6" t="s">
+        <v>412</v>
+      </c>
+      <c r="BP6" t="s">
+        <v>413</v>
+      </c>
+      <c r="BQ6" t="s">
+        <v>414</v>
+      </c>
+      <c r="BR6" t="s">
+        <v>415</v>
+      </c>
+      <c r="BS6" t="s">
+        <v>416</v>
+      </c>
+      <c r="BT6" t="s">
+        <v>417</v>
+      </c>
+      <c r="BU6" t="s">
+        <v>418</v>
+      </c>
+      <c r="BV6" t="s">
+        <v>419</v>
+      </c>
+      <c r="BW6" t="s">
+        <v>420</v>
+      </c>
+      <c r="BX6" t="s">
+        <v>421</v>
+      </c>
+      <c r="BY6" t="s">
+        <v>422</v>
+      </c>
+      <c r="BZ6" t="s">
+        <v>423</v>
+      </c>
+      <c r="CA6" t="s">
+        <v>424</v>
+      </c>
+      <c r="CB6" t="s">
+        <v>425</v>
+      </c>
+      <c r="CC6" t="s">
+        <v>426</v>
+      </c>
+      <c r="CD6" t="s">
+        <v>427</v>
+      </c>
+      <c r="CE6" t="s">
+        <v>428</v>
+      </c>
+      <c r="CF6" t="s">
+        <v>429</v>
+      </c>
+      <c r="CG6" t="s">
+        <v>430</v>
+      </c>
+      <c r="CH6" t="s">
+        <v>431</v>
+      </c>
+      <c r="CI6" t="s">
+        <v>432</v>
+      </c>
+      <c r="CJ6" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="CK6" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="CL6" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="CM6" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="CN6" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="Q6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="R6" s="11" t="s">
+      <c r="CO6" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="CP6" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="CQ6" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="CR6" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="V6" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="W6" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="X6" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="Y6" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z6" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="AA6" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="AB6" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="AC6" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="AD6" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="AE6" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="AF6" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="AG6" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="AH6" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="AI6" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="AJ6" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="AK6" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="AL6" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="AM6" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="AN6" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="AO6" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="AP6" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="AQ6" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="AR6" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="AS6" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="AT6" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="AU6" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV6" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="AW6" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="AX6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY6" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="AZ6" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="BA6" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="BB6" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="BC6" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="BD6" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="BE6" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="BF6" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="BG6" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="BH6" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="BI6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="BJ6" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="BK6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="BL6" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM6" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="BN6" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="BO6" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="BP6" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="BQ6" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="BR6" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="BT6" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="BU6" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="BV6" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="BW6" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="BX6" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="BY6" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="BZ6" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="CA6" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="CB6" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="CC6" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="CD6" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="CE6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="CF6" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="CG6" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="CH6" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="CI6" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="CJ6" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="CK6" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="CL6" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="CM6" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="CN6" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="CO6" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="CP6" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="CQ6" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="CR6" s="11" t="s">
-        <v>228</v>
       </c>
       <c r="CS6" s="13" t="s">
         <v>96</v>
@@ -5068,55 +5173,55 @@
         <v>104</v>
       </c>
       <c r="DB6" s="11" t="s">
-        <v>229</v>
+        <v>186</v>
       </c>
       <c r="DC6" s="11" t="s">
-        <v>230</v>
+        <v>187</v>
       </c>
       <c r="DD6" s="11" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="DE6" s="11" t="s">
-        <v>232</v>
+        <v>189</v>
       </c>
       <c r="DF6" s="11" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
       <c r="DG6" s="11" t="s">
         <v>109</v>
       </c>
       <c r="DH6" s="11" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
       <c r="DI6" s="14" t="s">
-        <v>235</v>
+        <v>192</v>
       </c>
       <c r="DJ6" s="11" t="s">
-        <v>236</v>
+        <v>193</v>
       </c>
       <c r="DK6" s="11" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="DL6" s="11" t="s">
         <v>114</v>
       </c>
       <c r="DM6" s="11" t="s">
-        <v>238</v>
+        <v>195</v>
       </c>
       <c r="DN6" s="11" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="DO6" s="11" t="s">
-        <v>240</v>
+        <v>197</v>
       </c>
       <c r="DP6" s="11" t="s">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="DQ6" s="11" t="s">
         <v>119</v>
       </c>
       <c r="DR6" s="11" t="s">
-        <v>242</v>
+        <v>199</v>
       </c>
       <c r="DS6" s="11" t="s">
         <v>121</v>
@@ -5125,7 +5230,7 @@
         <v>122</v>
       </c>
       <c r="DU6" s="11" t="s">
-        <v>243</v>
+        <v>200</v>
       </c>
       <c r="DV6" s="11" t="s">
         <v>124</v>
@@ -5161,7 +5266,7 @@
         <v>134</v>
       </c>
       <c r="EG6" s="13" t="s">
-        <v>244</v>
+        <v>201</v>
       </c>
       <c r="EH6" s="11" t="s">
         <v>136</v>
@@ -5170,13 +5275,13 @@
         <v>137</v>
       </c>
       <c r="EJ6" s="11" t="s">
-        <v>245</v>
+        <v>202</v>
       </c>
       <c r="EK6" s="11" t="s">
-        <v>246</v>
+        <v>203</v>
       </c>
       <c r="EL6" s="11" t="s">
-        <v>247</v>
+        <v>204</v>
       </c>
       <c r="EM6" s="13" t="s">
         <v>141</v>
@@ -5185,13 +5290,13 @@
         <v>142</v>
       </c>
       <c r="EO6" s="11" t="s">
-        <v>248</v>
+        <v>205</v>
       </c>
       <c r="EP6" s="11" t="s">
-        <v>249</v>
+        <v>206</v>
       </c>
       <c r="EQ6" s="11" t="s">
-        <v>250</v>
+        <v>207</v>
       </c>
       <c r="ER6" s="11" t="s">
         <v>146</v>
@@ -5215,37 +5320,37 @@
         <v>152</v>
       </c>
       <c r="EY6" s="14" t="s">
-        <v>251</v>
+        <v>208</v>
       </c>
       <c r="EZ6" s="14" t="s">
         <v>154</v>
       </c>
       <c r="FA6" s="11" t="s">
-        <v>252</v>
+        <v>209</v>
       </c>
       <c r="FB6" s="11" t="s">
         <v>156</v>
       </c>
       <c r="FC6" s="11" t="s">
-        <v>253</v>
+        <v>210</v>
       </c>
       <c r="FD6" s="11" t="s">
-        <v>254</v>
+        <v>211</v>
       </c>
       <c r="FE6" s="11" t="s">
         <v>159</v>
       </c>
       <c r="FF6" s="11" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="FG6" s="13" t="s">
-        <v>255</v>
+        <v>212</v>
       </c>
       <c r="FH6" s="15" t="s">
-        <v>256</v>
+        <v>213</v>
       </c>
       <c r="FI6" s="15" t="s">
-        <v>257</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -5269,27 +5374,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="48" t="s">
-        <v>318</v>
+        <v>275</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>319</v>
+        <v>276</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>320</v>
+        <v>277</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>321</v>
+        <v>278</v>
       </c>
       <c r="E1" s="48" t="s">
-        <v>322</v>
+        <v>279</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>323</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="49" t="s">
-        <v>324</v>
+        <v>281</v>
       </c>
       <c r="B2" s="49">
         <v>93.7</v>
@@ -5309,7 +5414,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="49" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="B3" s="49">
         <v>92.1</v>
@@ -5329,7 +5434,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="49" t="s">
-        <v>325</v>
+        <v>282</v>
       </c>
       <c r="B4" s="49">
         <v>91.8</v>
@@ -5349,7 +5454,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="49" t="s">
-        <v>326</v>
+        <v>283</v>
       </c>
       <c r="B5" s="49">
         <v>90.4</v>
@@ -5369,7 +5474,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="49" t="s">
-        <v>327</v>
+        <v>284</v>
       </c>
       <c r="B6" s="49">
         <v>93.7</v>
@@ -5414,39 +5519,39 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.6">
       <c r="A1" s="22" t="s">
-        <v>259</v>
+        <v>216</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>261</v>
+        <v>218</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>262</v>
+        <v>219</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>263</v>
+        <v>220</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>264</v>
+        <v>221</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>265</v>
+        <v>222</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>267</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18">
       <c r="A2" s="27" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>48</v>
@@ -5472,13 +5577,13 @@
     </row>
     <row r="3" spans="1:9" ht="18">
       <c r="A3" s="27" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>270</v>
+        <v>227</v>
       </c>
       <c r="D3" s="33">
         <v>0</v>
@@ -5501,10 +5606,10 @@
     </row>
     <row r="4" spans="1:9" ht="18">
       <c r="A4" s="27" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>40</v>
@@ -5530,10 +5635,10 @@
     </row>
     <row r="5" spans="1:9" ht="18">
       <c r="A5" s="27" t="s">
-        <v>271</v>
+        <v>228</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="C5" s="34" t="s">
         <v>12</v>
@@ -5559,10 +5664,10 @@
     </row>
     <row r="6" spans="1:9" ht="18">
       <c r="A6" s="27" t="s">
-        <v>271</v>
+        <v>228</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>8</v>
@@ -5588,10 +5693,10 @@
     </row>
     <row r="7" spans="1:9" ht="18">
       <c r="A7" s="27" t="s">
-        <v>271</v>
+        <v>228</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>10</v>
@@ -5617,10 +5722,10 @@
     </row>
     <row r="8" spans="1:9" ht="18">
       <c r="A8" s="27" t="s">
-        <v>272</v>
+        <v>229</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>2</v>
@@ -5646,10 +5751,10 @@
     </row>
     <row r="9" spans="1:9" ht="18">
       <c r="A9" s="27" t="s">
-        <v>272</v>
+        <v>229</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="C9" s="29" t="s">
         <v>56</v>
@@ -5675,10 +5780,10 @@
     </row>
     <row r="10" spans="1:9" ht="18">
       <c r="A10" s="27" t="s">
-        <v>273</v>
+        <v>230</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>97</v>
@@ -5704,10 +5809,10 @@
     </row>
     <row r="11" spans="1:9" ht="18">
       <c r="A11" s="27" t="s">
-        <v>273</v>
+        <v>230</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
       <c r="C11" s="36" t="s">
         <v>98</v>
@@ -5733,10 +5838,10 @@
     </row>
     <row r="12" spans="1:9" ht="18">
       <c r="A12" s="27" t="s">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C12" s="33" t="s">
         <v>57</v>
@@ -5762,10 +5867,10 @@
     </row>
     <row r="13" spans="1:9" ht="18">
       <c r="A13" s="27" t="s">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C13" s="33" t="s">
         <v>76</v>
@@ -5791,10 +5896,10 @@
     </row>
     <row r="14" spans="1:9" ht="18">
       <c r="A14" s="27" t="s">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>109</v>
@@ -5820,10 +5925,10 @@
     </row>
     <row r="15" spans="1:9" ht="18">
       <c r="A15" s="27" t="s">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C15" s="38" t="s">
         <v>99</v>
@@ -5849,10 +5954,10 @@
     </row>
     <row r="16" spans="1:9" ht="18">
       <c r="A16" s="27" t="s">
-        <v>276</v>
+        <v>233</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C16" s="29" t="s">
         <v>51</v>
@@ -5878,10 +5983,10 @@
     </row>
     <row r="17" spans="1:9" ht="18">
       <c r="A17" s="27" t="s">
-        <v>276</v>
+        <v>233</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C17" s="33" t="s">
         <v>20</v>
@@ -5907,10 +6012,10 @@
     </row>
     <row r="18" spans="1:9" ht="18">
       <c r="A18" s="27" t="s">
-        <v>276</v>
+        <v>233</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C18" s="35" t="s">
         <v>15</v>
@@ -5936,10 +6041,10 @@
     </row>
     <row r="19" spans="1:9" ht="18">
       <c r="A19" s="27" t="s">
-        <v>277</v>
+        <v>234</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>42</v>
@@ -5965,10 +6070,10 @@
     </row>
     <row r="20" spans="1:9" ht="18">
       <c r="A20" s="27" t="s">
-        <v>277</v>
+        <v>234</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C20" s="33" t="s">
         <v>33</v>
@@ -5994,10 +6099,10 @@
     </row>
     <row r="21" spans="1:9" ht="18">
       <c r="A21" s="27" t="s">
-        <v>277</v>
+        <v>234</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C21" s="33" t="s">
         <v>4</v>
@@ -6023,10 +6128,10 @@
     </row>
     <row r="22" spans="1:9" ht="18">
       <c r="A22" s="27" t="s">
-        <v>277</v>
+        <v>234</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C22" s="39" t="s">
         <v>88</v>
@@ -6052,10 +6157,10 @@
     </row>
     <row r="23" spans="1:9" ht="18">
       <c r="A23" s="27" t="s">
-        <v>278</v>
+        <v>235</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C23" s="34" t="s">
         <v>52</v>
@@ -6081,10 +6186,10 @@
     </row>
     <row r="24" spans="1:9" ht="18">
       <c r="A24" s="27" t="s">
-        <v>279</v>
+        <v>236</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C24" s="35" t="s">
         <v>91</v>
@@ -6110,13 +6215,13 @@
     </row>
     <row r="25" spans="1:9" ht="18">
       <c r="A25" s="27" t="s">
-        <v>279</v>
+        <v>236</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>275</v>
+        <v>232</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>270</v>
+        <v>227</v>
       </c>
       <c r="D25" s="33">
         <v>0</v>
@@ -6139,10 +6244,10 @@
     </row>
     <row r="26" spans="1:9" ht="18">
       <c r="A26" s="27" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="C26" s="29" t="s">
         <v>8</v>
@@ -6168,10 +6273,10 @@
     </row>
     <row r="27" spans="1:9" ht="18">
       <c r="A27" s="27" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="C27" s="34" t="s">
         <v>12</v>
@@ -6197,10 +6302,10 @@
     </row>
     <row r="28" spans="1:9" ht="18">
       <c r="A28" s="27" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="C28" s="29" t="s">
         <v>11</v>
@@ -6226,10 +6331,10 @@
     </row>
     <row r="29" spans="1:9" ht="18">
       <c r="A29" s="27" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="C29" s="41" t="s">
         <v>21</v>
@@ -6255,10 +6360,10 @@
     </row>
     <row r="30" spans="1:9" ht="18">
       <c r="A30" s="27" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>22</v>
@@ -6284,10 +6389,10 @@
     </row>
     <row r="31" spans="1:9" ht="18">
       <c r="A31" s="27" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="C31" s="35" t="s">
         <v>10</v>
@@ -6313,10 +6418,10 @@
     </row>
     <row r="32" spans="1:9" ht="18">
       <c r="A32" s="27" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="C32" s="29" t="s">
         <v>94</v>
@@ -6342,13 +6447,13 @@
     </row>
     <row r="33" spans="1:9" ht="18">
       <c r="A33" s="27" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>283</v>
+        <v>240</v>
       </c>
       <c r="D33" s="29">
         <v>1</v>
@@ -6371,10 +6476,10 @@
     </row>
     <row r="34" spans="1:9" ht="18">
       <c r="A34" s="27" t="s">
-        <v>284</v>
+        <v>241</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C34" s="29" t="s">
         <v>94</v>
@@ -6400,10 +6505,10 @@
     </row>
     <row r="35" spans="1:9" ht="18">
       <c r="A35" s="27" t="s">
-        <v>284</v>
+        <v>241</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C35" s="35" t="s">
         <v>110</v>
@@ -6429,13 +6534,13 @@
     </row>
     <row r="36" spans="1:9" ht="18">
       <c r="A36" s="27" t="s">
-        <v>284</v>
+        <v>241</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>283</v>
+        <v>240</v>
       </c>
       <c r="D36" s="29">
         <v>1</v>
@@ -6458,10 +6563,10 @@
     </row>
     <row r="37" spans="1:9" ht="18">
       <c r="A37" s="27" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C37" s="29" t="s">
         <v>48</v>
@@ -6487,10 +6592,10 @@
     </row>
     <row r="38" spans="1:9" ht="18">
       <c r="A38" s="27" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>40</v>
@@ -6516,10 +6621,10 @@
     </row>
     <row r="39" spans="1:9" ht="18">
       <c r="A39" s="27" t="s">
-        <v>286</v>
+        <v>243</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C39" s="35" t="s">
         <v>96</v>
@@ -6545,10 +6650,10 @@
     </row>
     <row r="40" spans="1:9" ht="18">
       <c r="A40" s="27" t="s">
-        <v>286</v>
+        <v>243</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C40" s="29" t="s">
         <v>97</v>
@@ -6574,10 +6679,10 @@
     </row>
     <row r="41" spans="1:9" ht="18">
       <c r="A41" s="27" t="s">
-        <v>287</v>
+        <v>244</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C41" s="35" t="s">
         <v>15</v>
@@ -6603,10 +6708,10 @@
     </row>
     <row r="42" spans="1:9" ht="18">
       <c r="A42" s="27" t="s">
-        <v>287</v>
+        <v>244</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C42" s="33" t="s">
         <v>20</v>
@@ -6632,10 +6737,10 @@
     </row>
     <row r="43" spans="1:9" ht="18">
       <c r="A43" s="27" t="s">
-        <v>287</v>
+        <v>244</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C43" s="29" t="s">
         <v>51</v>
@@ -6661,10 +6766,10 @@
     </row>
     <row r="44" spans="1:9" ht="18">
       <c r="A44" s="27" t="s">
-        <v>288</v>
+        <v>245</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C44" s="29" t="s">
         <v>2</v>
@@ -6690,10 +6795,10 @@
     </row>
     <row r="45" spans="1:9" ht="18">
       <c r="A45" s="27" t="s">
-        <v>288</v>
+        <v>245</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>285</v>
+        <v>242</v>
       </c>
       <c r="C45" s="29" t="s">
         <v>49</v>
@@ -6719,10 +6824,10 @@
     </row>
     <row r="46" spans="1:9" ht="18">
       <c r="A46" s="27" t="s">
-        <v>289</v>
+        <v>246</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="C46" s="29" t="s">
         <v>94</v>
@@ -6748,10 +6853,10 @@
     </row>
     <row r="47" spans="1:9" ht="18">
       <c r="A47" s="27" t="s">
-        <v>289</v>
+        <v>246</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="C47" s="35" t="s">
         <v>110</v>
@@ -6777,13 +6882,13 @@
     </row>
     <row r="48" spans="1:9" ht="18">
       <c r="A48" s="27" t="s">
-        <v>289</v>
+        <v>246</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>283</v>
+        <v>240</v>
       </c>
       <c r="D48" s="29">
         <v>1</v>
@@ -6806,10 +6911,10 @@
     </row>
     <row r="49" spans="1:9" ht="18">
       <c r="A49" s="27" t="s">
-        <v>290</v>
+        <v>247</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="C49" s="33" t="s">
         <v>20</v>
@@ -6835,10 +6940,10 @@
     </row>
     <row r="50" spans="1:9" ht="18">
       <c r="A50" s="27" t="s">
-        <v>290</v>
+        <v>247</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="C50" s="29" t="s">
         <v>6</v>
@@ -6864,10 +6969,10 @@
     </row>
     <row r="51" spans="1:9" ht="18">
       <c r="A51" s="27" t="s">
-        <v>291</v>
+        <v>248</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="C51" s="29" t="s">
         <v>8</v>
@@ -6893,10 +6998,10 @@
     </row>
     <row r="52" spans="1:9" ht="18">
       <c r="A52" s="27" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="C52" s="29" t="s">
         <v>51</v>
@@ -6922,10 +7027,10 @@
     </row>
     <row r="53" spans="1:9" ht="18">
       <c r="A53" s="27" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="C53" s="29" t="s">
         <v>2</v>
@@ -6951,10 +7056,10 @@
     </row>
     <row r="54" spans="1:9" ht="18">
       <c r="A54" s="27" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="C54" s="29" t="s">
         <v>18</v>
@@ -6980,10 +7085,10 @@
     </row>
     <row r="55" spans="1:9" ht="18">
       <c r="A55" s="27" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="C55" s="29" t="s">
         <v>8</v>
@@ -7009,10 +7114,10 @@
     </row>
     <row r="56" spans="1:9" ht="18">
       <c r="A56" s="27" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="B56" s="28" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="C56" s="33" t="s">
         <v>17</v>
@@ -7038,10 +7143,10 @@
     </row>
     <row r="57" spans="1:9" ht="18">
       <c r="A57" s="27" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="B57" s="28" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="C57" s="29" t="s">
         <v>5</v>
@@ -7067,10 +7172,10 @@
     </row>
     <row r="58" spans="1:9" ht="18">
       <c r="A58" s="27" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="C58" s="33" t="s">
         <v>4</v>
@@ -7096,10 +7201,10 @@
     </row>
     <row r="59" spans="1:9" ht="18">
       <c r="A59" s="27" t="s">
-        <v>296</v>
+        <v>253</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="C59" s="29" t="s">
         <v>48</v>
@@ -7123,10 +7228,10 @@
     </row>
     <row r="60" spans="1:9" ht="18">
       <c r="A60" s="27" t="s">
-        <v>296</v>
+        <v>253</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="C60" s="33" t="s">
         <v>40</v>
@@ -7152,10 +7257,10 @@
     </row>
     <row r="61" spans="1:9" ht="18">
       <c r="A61" s="27" t="s">
-        <v>272</v>
+        <v>229</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="C61" s="29" t="s">
         <v>56</v>
@@ -7181,10 +7286,10 @@
     </row>
     <row r="62" spans="1:9" ht="18">
       <c r="A62" s="27" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="C62" s="33" t="s">
         <v>57</v>
@@ -7210,10 +7315,10 @@
     </row>
     <row r="63" spans="1:9" ht="18">
       <c r="A63" s="27" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="C63" s="33" t="s">
         <v>76</v>
@@ -7239,10 +7344,10 @@
     </row>
     <row r="64" spans="1:9" ht="18">
       <c r="A64" s="27" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="C64" s="34" t="s">
         <v>109</v>
@@ -7268,10 +7373,10 @@
     </row>
     <row r="65" spans="1:9" ht="18">
       <c r="A65" s="27" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="C65" s="38" t="s">
         <v>99</v>
@@ -7297,10 +7402,10 @@
     </row>
     <row r="66" spans="1:9" ht="18">
       <c r="A66" s="27" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="C66" s="35" t="s">
         <v>96</v>
@@ -7326,10 +7431,10 @@
     </row>
     <row r="67" spans="1:9" ht="18">
       <c r="A67" s="27" t="s">
-        <v>299</v>
+        <v>256</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="C67" s="29" t="s">
         <v>97</v>
@@ -7355,10 +7460,10 @@
     </row>
     <row r="68" spans="1:9" ht="18">
       <c r="A68" s="27" t="s">
-        <v>299</v>
+        <v>256</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="C68" s="36" t="s">
         <v>98</v>
@@ -7384,10 +7489,10 @@
     </row>
     <row r="69" spans="1:9" ht="18">
       <c r="A69" s="27" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="C69" s="29" t="s">
         <v>48</v>
@@ -7413,10 +7518,10 @@
     </row>
     <row r="70" spans="1:9" ht="18">
       <c r="A70" s="27" t="s">
-        <v>301</v>
+        <v>258</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="C70" s="29" t="s">
         <v>18</v>
@@ -7442,10 +7547,10 @@
     </row>
     <row r="71" spans="1:9" ht="18">
       <c r="A71" s="27" t="s">
-        <v>302</v>
+        <v>259</v>
       </c>
       <c r="B71" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C71" s="35" t="s">
         <v>55</v>
@@ -7471,10 +7576,10 @@
     </row>
     <row r="72" spans="1:9" ht="18">
       <c r="A72" s="27" t="s">
-        <v>302</v>
+        <v>259</v>
       </c>
       <c r="B72" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C72" s="35" t="s">
         <v>91</v>
@@ -7500,10 +7605,10 @@
     </row>
     <row r="73" spans="1:9" ht="18">
       <c r="A73" s="27" t="s">
-        <v>304</v>
+        <v>261</v>
       </c>
       <c r="B73" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C73" s="29" t="s">
         <v>54</v>
@@ -7529,10 +7634,10 @@
     </row>
     <row r="74" spans="1:9" ht="18">
       <c r="A74" s="27" t="s">
-        <v>305</v>
+        <v>262</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C74" s="29" t="s">
         <v>14</v>
@@ -7558,10 +7663,10 @@
     </row>
     <row r="75" spans="1:9" ht="18">
       <c r="A75" s="27" t="s">
-        <v>305</v>
+        <v>262</v>
       </c>
       <c r="B75" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C75" s="22" t="s">
         <v>111</v>
@@ -7587,10 +7692,10 @@
     </row>
     <row r="76" spans="1:9" ht="18">
       <c r="A76" s="27" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
       <c r="B76" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C76" s="33" t="s">
         <v>47</v>
@@ -7616,10 +7721,10 @@
     </row>
     <row r="77" spans="1:9" ht="18">
       <c r="A77" s="27" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
       <c r="B77" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C77" s="29" t="s">
         <v>48</v>
@@ -7645,10 +7750,10 @@
     </row>
     <row r="78" spans="1:9" ht="18">
       <c r="A78" s="27" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C78" s="33" t="s">
         <v>95</v>
@@ -7674,10 +7779,10 @@
     </row>
     <row r="79" spans="1:9" ht="18">
       <c r="A79" s="27" t="s">
-        <v>307</v>
+        <v>264</v>
       </c>
       <c r="B79" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C79" s="29" t="s">
         <v>18</v>
@@ -7703,10 +7808,10 @@
     </row>
     <row r="80" spans="1:9" ht="18">
       <c r="A80" s="27" t="s">
-        <v>307</v>
+        <v>264</v>
       </c>
       <c r="B80" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C80" s="35" t="s">
         <v>110</v>
@@ -7732,10 +7837,10 @@
     </row>
     <row r="81" spans="1:9" ht="18">
       <c r="A81" s="27" t="s">
-        <v>308</v>
+        <v>265</v>
       </c>
       <c r="B81" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C81" s="22" t="s">
         <v>120</v>
@@ -7761,10 +7866,10 @@
     </row>
     <row r="82" spans="1:9" ht="18">
       <c r="A82" s="27" t="s">
-        <v>309</v>
+        <v>266</v>
       </c>
       <c r="B82" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C82" s="33" t="s">
         <v>76</v>
@@ -7790,10 +7895,10 @@
     </row>
     <row r="83" spans="1:9" ht="18">
       <c r="A83" s="27" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="B83" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C83" s="33" t="s">
         <v>42</v>
@@ -7819,10 +7924,10 @@
     </row>
     <row r="84" spans="1:9" ht="18">
       <c r="A84" s="27" t="s">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="B84" s="28" t="s">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="C84" s="33" t="s">
         <v>22</v>
@@ -7848,10 +7953,10 @@
     </row>
     <row r="85" spans="1:9" ht="18">
       <c r="A85" s="27" t="s">
-        <v>311</v>
+        <v>268</v>
       </c>
       <c r="B85" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C85" s="29" t="s">
         <v>94</v>
@@ -7877,10 +7982,10 @@
     </row>
     <row r="86" spans="1:9" ht="18">
       <c r="A86" s="27" t="s">
-        <v>311</v>
+        <v>268</v>
       </c>
       <c r="B86" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C86" s="29" t="s">
         <v>18</v>
@@ -7906,13 +8011,13 @@
     </row>
     <row r="87" spans="1:9" ht="18">
       <c r="A87" s="27" t="s">
-        <v>311</v>
+        <v>268</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C87" s="29" t="s">
-        <v>283</v>
+        <v>240</v>
       </c>
       <c r="D87" s="29">
         <v>1</v>
@@ -7935,10 +8040,10 @@
     </row>
     <row r="88" spans="1:9" ht="18">
       <c r="A88" s="27" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="B88" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C88" s="29" t="s">
         <v>48</v>
@@ -7964,10 +8069,10 @@
     </row>
     <row r="89" spans="1:9" ht="18">
       <c r="A89" s="27" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="B89" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C89" s="22" t="s">
         <v>114</v>
@@ -7993,10 +8098,10 @@
     </row>
     <row r="90" spans="1:9" ht="18">
       <c r="A90" s="27" t="s">
-        <v>313</v>
+        <v>270</v>
       </c>
       <c r="B90" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C90" s="33" t="s">
         <v>95</v>
@@ -8022,10 +8127,10 @@
     </row>
     <row r="91" spans="1:9" ht="18">
       <c r="A91" s="27" t="s">
-        <v>313</v>
+        <v>270</v>
       </c>
       <c r="B91" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C91" s="22" t="s">
         <v>115</v>
@@ -8051,10 +8156,10 @@
     </row>
     <row r="92" spans="1:9" ht="18">
       <c r="A92" s="27" t="s">
-        <v>314</v>
+        <v>271</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C92" s="35" t="s">
         <v>10</v>
@@ -8080,10 +8185,10 @@
     </row>
     <row r="93" spans="1:9" ht="18">
       <c r="A93" s="27" t="s">
-        <v>314</v>
+        <v>271</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C93" s="34" t="s">
         <v>12</v>
@@ -8109,10 +8214,10 @@
     </row>
     <row r="94" spans="1:9" ht="18">
       <c r="A94" s="27" t="s">
-        <v>314</v>
+        <v>271</v>
       </c>
       <c r="B94" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C94" s="29" t="s">
         <v>8</v>
@@ -8138,10 +8243,10 @@
     </row>
     <row r="95" spans="1:9" ht="18">
       <c r="A95" s="27" t="s">
-        <v>315</v>
+        <v>272</v>
       </c>
       <c r="B95" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C95" s="35" t="s">
         <v>91</v>
@@ -8167,10 +8272,10 @@
     </row>
     <row r="96" spans="1:9" ht="18">
       <c r="A96" s="27" t="s">
-        <v>316</v>
+        <v>273</v>
       </c>
       <c r="B96" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C96" s="33" t="s">
         <v>20</v>
@@ -8196,10 +8301,10 @@
     </row>
     <row r="97" spans="1:9" ht="18">
       <c r="A97" s="27" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
       <c r="B97" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C97" s="41" t="s">
         <v>21</v>
@@ -8225,10 +8330,10 @@
     </row>
     <row r="98" spans="1:9" ht="18">
       <c r="A98" s="27" t="s">
-        <v>317</v>
+        <v>274</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>312</v>
+        <v>269</v>
       </c>
       <c r="C98" s="35" t="s">
         <v>15</v>
@@ -8386,10 +8491,10 @@
   <sheetData>
     <row r="1" spans="1:166">
       <c r="A1" s="51" t="s">
-        <v>328</v>
+        <v>285</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="C1" s="51" t="s">
         <v>1</v>
@@ -8710,7 +8815,7 @@
         <v>106</v>
       </c>
       <c r="DE1" s="51" t="s">
-        <v>270</v>
+        <v>227</v>
       </c>
       <c r="DF1" s="51" t="s">
         <v>107</v>
@@ -8886,10 +8991,10 @@
     </row>
     <row r="2" spans="1:166" ht="15.6">
       <c r="A2" s="50" t="s">
-        <v>330</v>
+        <v>287</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C2" s="50">
         <v>0.11170740773016183</v>
@@ -9388,10 +9493,10 @@
     </row>
     <row r="3" spans="1:166" ht="15.6">
       <c r="A3" s="50" t="s">
-        <v>332</v>
+        <v>289</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C3" s="50">
         <v>6.3228645007263856E-2</v>
@@ -9890,10 +9995,10 @@
     </row>
     <row r="4" spans="1:166" ht="15.6">
       <c r="A4" s="50" t="s">
-        <v>333</v>
+        <v>290</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C4" s="50">
         <v>0.10636939054225673</v>
@@ -10392,10 +10497,10 @@
     </row>
     <row r="5" spans="1:166" ht="15.6">
       <c r="A5" s="50" t="s">
-        <v>334</v>
+        <v>291</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C5" s="50">
         <v>0.1461566504185623</v>
@@ -10894,10 +10999,10 @@
     </row>
     <row r="6" spans="1:166" ht="15.6">
       <c r="A6" s="50" t="s">
-        <v>335</v>
+        <v>292</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C6" s="50">
         <v>0.12043559926698584</v>
@@ -11396,10 +11501,10 @@
     </row>
     <row r="7" spans="1:166" ht="15.6">
       <c r="A7" s="50" t="s">
-        <v>336</v>
+        <v>293</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C7" s="50">
         <v>5.443753888220583E-2</v>
@@ -11898,10 +12003,10 @@
     </row>
     <row r="8" spans="1:166" ht="15.6">
       <c r="A8" s="50" t="s">
-        <v>337</v>
+        <v>294</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C8" s="50">
         <v>0.17510680398775119</v>
@@ -12400,10 +12505,10 @@
     </row>
     <row r="9" spans="1:166" ht="15.6">
       <c r="A9" s="50" t="s">
-        <v>338</v>
+        <v>295</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C9" s="50">
         <v>0.10527742596547907</v>
@@ -12902,10 +13007,10 @@
     </row>
     <row r="10" spans="1:166" ht="15.6">
       <c r="A10" s="50" t="s">
-        <v>339</v>
+        <v>296</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C10" s="50">
         <v>9.6046310784620142E-2</v>
@@ -13404,10 +13509,10 @@
     </row>
     <row r="11" spans="1:166" ht="15.6">
       <c r="A11" s="50" t="s">
-        <v>340</v>
+        <v>297</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C11" s="50">
         <v>0.11778898006790711</v>
@@ -13906,10 +14011,10 @@
     </row>
     <row r="12" spans="1:166" ht="15.6">
       <c r="A12" s="50" t="s">
-        <v>341</v>
+        <v>298</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C12" s="50">
         <v>0.13596736298054929</v>
@@ -14408,10 +14513,10 @@
     </row>
     <row r="13" spans="1:166" ht="15.6">
       <c r="A13" s="50" t="s">
-        <v>342</v>
+        <v>299</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C13" s="50">
         <v>0.21902021475901565</v>
@@ -14910,10 +15015,10 @@
     </row>
     <row r="14" spans="1:166" ht="15.6">
       <c r="A14" s="50" t="s">
-        <v>343</v>
+        <v>300</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C14" s="50">
         <v>9.8741557137914771E-2</v>
@@ -15412,10 +15517,10 @@
     </row>
     <row r="15" spans="1:166" ht="15.6">
       <c r="A15" s="50" t="s">
-        <v>344</v>
+        <v>301</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C15" s="50">
         <v>0.11372400316099249</v>
@@ -15914,10 +16019,10 @@
     </row>
     <row r="16" spans="1:166" ht="15.6">
       <c r="A16" s="50" t="s">
-        <v>345</v>
+        <v>302</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C16" s="50">
         <v>9.628698969422804E-2</v>
@@ -16416,10 +16521,10 @@
     </row>
     <row r="17" spans="1:166" ht="15.6">
       <c r="A17" s="50" t="s">
-        <v>346</v>
+        <v>303</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C17" s="50">
         <v>0.1100956732486822</v>
@@ -16918,10 +17023,10 @@
     </row>
     <row r="18" spans="1:166" ht="15.6">
       <c r="A18" s="50" t="s">
-        <v>347</v>
+        <v>304</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C18" s="50">
         <v>0.15091731358750016</v>
@@ -17420,10 +17525,10 @@
     </row>
     <row r="19" spans="1:166" ht="15.6">
       <c r="A19" s="50" t="s">
-        <v>348</v>
+        <v>305</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C19" s="50">
         <v>0.15634917240727847</v>
@@ -17922,10 +18027,10 @@
     </row>
     <row r="20" spans="1:166" ht="15.6">
       <c r="A20" s="50" t="s">
-        <v>349</v>
+        <v>306</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C20" s="50">
         <v>0.26466963572319374</v>
@@ -18424,10 +18529,10 @@
     </row>
     <row r="21" spans="1:166" ht="15.6">
       <c r="A21" s="50" t="s">
-        <v>350</v>
+        <v>307</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C21" s="50">
         <v>0.14356805683774243</v>
@@ -18926,10 +19031,10 @@
     </row>
     <row r="22" spans="1:166" ht="15.6">
       <c r="A22" s="50" t="s">
-        <v>351</v>
+        <v>308</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C22" s="50">
         <v>0.12027504255172759</v>
@@ -19428,10 +19533,10 @@
     </row>
     <row r="23" spans="1:166" ht="15.6">
       <c r="A23" s="50" t="s">
-        <v>352</v>
+        <v>309</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C23" s="50">
         <v>0.11617150229872404</v>
@@ -19930,10 +20035,10 @@
     </row>
     <row r="24" spans="1:166" ht="15.6">
       <c r="A24" s="50" t="s">
-        <v>353</v>
+        <v>310</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C24" s="50">
         <v>0.10819057311318168</v>
@@ -20432,10 +20537,10 @@
     </row>
     <row r="25" spans="1:166" ht="15.6">
       <c r="A25" s="50" t="s">
-        <v>354</v>
+        <v>311</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C25" s="50">
         <v>0.14061251239896741</v>
@@ -20934,10 +21039,10 @@
     </row>
     <row r="26" spans="1:166" ht="15.6">
       <c r="A26" s="50" t="s">
-        <v>355</v>
+        <v>312</v>
       </c>
       <c r="B26" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C26" s="50">
         <v>0.14427494166901061</v>
@@ -21436,10 +21541,10 @@
     </row>
     <row r="27" spans="1:166" ht="15.6">
       <c r="A27" s="50" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C27" s="50">
         <v>0.15470809467981528</v>
@@ -21938,10 +22043,10 @@
     </row>
     <row r="28" spans="1:166" ht="15.6">
       <c r="A28" s="50" t="s">
-        <v>357</v>
+        <v>314</v>
       </c>
       <c r="B28" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C28" s="50">
         <v>0.12570280552655935</v>
@@ -22440,10 +22545,10 @@
     </row>
     <row r="29" spans="1:166" ht="15.6">
       <c r="A29" s="50" t="s">
-        <v>358</v>
+        <v>315</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C29" s="50">
         <v>9.9351267577107868E-2</v>
@@ -22942,10 +23047,10 @@
     </row>
     <row r="30" spans="1:166" ht="15.6">
       <c r="A30" s="50" t="s">
-        <v>359</v>
+        <v>316</v>
       </c>
       <c r="B30" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C30" s="50">
         <v>0.11709383964483638</v>
@@ -23444,10 +23549,10 @@
     </row>
     <row r="31" spans="1:166" ht="15.6">
       <c r="A31" s="50" t="s">
-        <v>360</v>
+        <v>317</v>
       </c>
       <c r="B31" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C31" s="50">
         <v>0.14944495877423042</v>
@@ -23946,10 +24051,10 @@
     </row>
     <row r="32" spans="1:166" ht="15.6">
       <c r="A32" s="50" t="s">
-        <v>361</v>
+        <v>318</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C32" s="50">
         <v>0.16638250516345557</v>
@@ -24448,10 +24553,10 @@
     </row>
     <row r="33" spans="1:166" ht="15.6">
       <c r="A33" s="50" t="s">
-        <v>362</v>
+        <v>319</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C33" s="50">
         <v>0.17183964013669092</v>
@@ -24950,10 +25055,10 @@
     </row>
     <row r="34" spans="1:166" ht="15.6">
       <c r="A34" s="50" t="s">
-        <v>363</v>
+        <v>320</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C34" s="50">
         <v>9.9999638616400793E-2</v>
@@ -25452,10 +25557,10 @@
     </row>
     <row r="35" spans="1:166" ht="15.6">
       <c r="A35" s="50" t="s">
-        <v>364</v>
+        <v>321</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C35" s="50">
         <v>0.12736876385388857</v>
@@ -25954,10 +26059,10 @@
     </row>
     <row r="36" spans="1:166" ht="15.6">
       <c r="A36" s="50" t="s">
-        <v>365</v>
+        <v>322</v>
       </c>
       <c r="B36" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C36" s="50">
         <v>7.9712871637648827E-2</v>
@@ -26456,10 +26561,10 @@
     </row>
     <row r="37" spans="1:166" ht="15.6">
       <c r="A37" s="50" t="s">
-        <v>366</v>
+        <v>323</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C37" s="50">
         <v>0.13730604156633705</v>
@@ -26958,10 +27063,10 @@
     </row>
     <row r="38" spans="1:166" ht="15.6">
       <c r="A38" s="50" t="s">
-        <v>367</v>
+        <v>324</v>
       </c>
       <c r="B38" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C38" s="50">
         <v>0.1114143423882511</v>
@@ -27460,10 +27565,10 @@
     </row>
     <row r="39" spans="1:166" ht="15.6">
       <c r="A39" s="50" t="s">
-        <v>368</v>
+        <v>325</v>
       </c>
       <c r="B39" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C39" s="50">
         <v>0.12258852511297573</v>
@@ -27962,10 +28067,10 @@
     </row>
     <row r="40" spans="1:166" ht="15.6">
       <c r="A40" s="50" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
       <c r="B40" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C40" s="50">
         <v>9.1960364772645284E-2</v>
@@ -28464,10 +28569,10 @@
     </row>
     <row r="41" spans="1:166" ht="15.6">
       <c r="A41" s="50" t="s">
-        <v>370</v>
+        <v>327</v>
       </c>
       <c r="B41" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C41" s="50">
         <v>0.15016922306544853</v>
@@ -28966,10 +29071,10 @@
     </row>
     <row r="42" spans="1:166" ht="15.6">
       <c r="A42" s="50" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C42" s="50">
         <v>0.13206722782078495</v>
@@ -29468,10 +29573,10 @@
     </row>
     <row r="43" spans="1:166" ht="15.6">
       <c r="A43" s="50" t="s">
-        <v>372</v>
+        <v>329</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C43" s="50">
         <v>0.16095009969464044</v>
@@ -29970,10 +30075,10 @@
     </row>
     <row r="44" spans="1:166" ht="15.6">
       <c r="A44" s="50" t="s">
-        <v>373</v>
+        <v>330</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C44" s="50">
         <v>0.13421604403236001</v>
@@ -30472,10 +30577,10 @@
     </row>
     <row r="45" spans="1:166" ht="15.6">
       <c r="A45" s="50" t="s">
-        <v>374</v>
+        <v>331</v>
       </c>
       <c r="B45" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C45" s="50">
         <v>0.12680797744472594</v>
@@ -30974,10 +31079,10 @@
     </row>
     <row r="46" spans="1:166" ht="15.6">
       <c r="A46" s="50" t="s">
-        <v>375</v>
+        <v>332</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C46" s="50">
         <v>9.2254291122886384E-2</v>
@@ -31476,10 +31581,10 @@
     </row>
     <row r="47" spans="1:166" ht="15.6">
       <c r="A47" s="50" t="s">
-        <v>376</v>
+        <v>333</v>
       </c>
       <c r="B47" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C47" s="50">
         <v>0.1316438116461901</v>
@@ -31978,10 +32083,10 @@
     </row>
     <row r="48" spans="1:166" ht="15.6">
       <c r="A48" s="50" t="s">
-        <v>377</v>
+        <v>334</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C48" s="50">
         <v>0.10983066086961674</v>
@@ -32480,10 +32585,10 @@
     </row>
     <row r="49" spans="1:166" ht="15.6">
       <c r="A49" s="50" t="s">
-        <v>378</v>
+        <v>335</v>
       </c>
       <c r="B49" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C49" s="50">
         <v>0.16568871808072991</v>
@@ -32982,10 +33087,10 @@
     </row>
     <row r="50" spans="1:166" ht="15.6">
       <c r="A50" s="50" t="s">
-        <v>379</v>
+        <v>336</v>
       </c>
       <c r="B50" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C50" s="50">
         <v>0.12852349194599791</v>
@@ -33484,10 +33589,10 @@
     </row>
     <row r="51" spans="1:166" ht="15.6">
       <c r="A51" s="50" t="s">
-        <v>380</v>
+        <v>337</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C51" s="50">
         <v>0.12463980802036866</v>
@@ -33986,10 +34091,10 @@
     </row>
     <row r="52" spans="1:166" ht="15.6">
       <c r="A52" s="50" t="s">
-        <v>381</v>
+        <v>338</v>
       </c>
       <c r="B52" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C52" s="50">
         <v>0.10184789635679652</v>
@@ -34488,10 +34593,10 @@
     </row>
     <row r="53" spans="1:166" ht="15.6">
       <c r="A53" s="50" t="s">
-        <v>382</v>
+        <v>339</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C53" s="50">
         <v>0.14738836055623325</v>
@@ -34990,10 +35095,10 @@
     </row>
     <row r="54" spans="1:166" ht="15.6">
       <c r="A54" s="50" t="s">
-        <v>383</v>
+        <v>340</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C54" s="50">
         <v>0.14637778882801292</v>
@@ -35492,10 +35597,10 @@
     </row>
     <row r="55" spans="1:166" ht="15.6">
       <c r="A55" s="50" t="s">
-        <v>384</v>
+        <v>341</v>
       </c>
       <c r="B55" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C55" s="50">
         <v>0.15758282427497819</v>
@@ -35994,10 +36099,10 @@
     </row>
     <row r="56" spans="1:166" ht="15.6">
       <c r="A56" s="50" t="s">
-        <v>385</v>
+        <v>342</v>
       </c>
       <c r="B56" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C56" s="50">
         <v>0.16040543911079896</v>
@@ -36496,10 +36601,10 @@
     </row>
     <row r="57" spans="1:166" ht="15.6">
       <c r="A57" s="50" t="s">
-        <v>386</v>
+        <v>343</v>
       </c>
       <c r="B57" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C57" s="50">
         <v>0.17683485346003747</v>
@@ -36998,10 +37103,10 @@
     </row>
     <row r="58" spans="1:166" ht="15.6">
       <c r="A58" s="50" t="s">
-        <v>387</v>
+        <v>344</v>
       </c>
       <c r="B58" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C58" s="50">
         <v>0.31378757147679348</v>
@@ -37500,10 +37605,10 @@
     </row>
     <row r="59" spans="1:166" ht="15.6">
       <c r="A59" s="50" t="s">
-        <v>388</v>
+        <v>345</v>
       </c>
       <c r="B59" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C59" s="50">
         <v>0.19166009028142042</v>
@@ -38002,10 +38107,10 @@
     </row>
     <row r="60" spans="1:166" ht="15.6">
       <c r="A60" s="50" t="s">
-        <v>389</v>
+        <v>346</v>
       </c>
       <c r="B60" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C60" s="50">
         <v>5.8178703950426104E-2</v>
@@ -38504,10 +38609,10 @@
     </row>
     <row r="61" spans="1:166" ht="15.6">
       <c r="A61" s="50" t="s">
-        <v>390</v>
+        <v>347</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C61" s="50">
         <v>0.17782348965585196</v>
@@ -39006,10 +39111,10 @@
     </row>
     <row r="62" spans="1:166" ht="15.6">
       <c r="A62" s="50" t="s">
-        <v>391</v>
+        <v>348</v>
       </c>
       <c r="B62" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C62" s="50">
         <v>9.8477549993772506E-2</v>
@@ -39508,10 +39613,10 @@
     </row>
     <row r="63" spans="1:166" ht="15.6">
       <c r="A63" s="50" t="s">
-        <v>392</v>
+        <v>349</v>
       </c>
       <c r="B63" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C63" s="50">
         <v>0.11571392574598803</v>
@@ -40010,10 +40115,10 @@
     </row>
     <row r="64" spans="1:166" ht="15.6">
       <c r="A64" s="50" t="s">
-        <v>393</v>
+        <v>350</v>
       </c>
       <c r="B64" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C64" s="50">
         <v>0.11417833301723149</v>
@@ -40512,10 +40617,10 @@
     </row>
     <row r="65" spans="1:166" ht="15.6">
       <c r="A65" s="50" t="s">
-        <v>394</v>
+        <v>351</v>
       </c>
       <c r="B65" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C65" s="50">
         <v>0.10034903675451509</v>
@@ -41014,10 +41119,10 @@
     </row>
     <row r="66" spans="1:166" ht="15.6">
       <c r="A66" s="50" t="s">
-        <v>395</v>
+        <v>352</v>
       </c>
       <c r="B66" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C66" s="50">
         <v>0.16826182143477877</v>
@@ -41516,10 +41621,10 @@
     </row>
     <row r="67" spans="1:166" ht="15.6">
       <c r="A67" s="50" t="s">
-        <v>396</v>
+        <v>353</v>
       </c>
       <c r="B67" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C67" s="50">
         <v>0.13844840120575497</v>
@@ -42018,10 +42123,10 @@
     </row>
     <row r="68" spans="1:166" ht="15.6">
       <c r="A68" s="50" t="s">
-        <v>397</v>
+        <v>354</v>
       </c>
       <c r="B68" s="50" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="C68" s="50">
         <v>0.16291431512100477</v>

</xml_diff>